<commit_message>
Added combo and coop cards
</commit_message>
<xml_diff>
--- a/data/all-player-decks.xlsx
+++ b/data/all-player-decks.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nathan\Google Drive\Projects\Raspberry\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Google Drive\Projects\Raspberry\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18975" windowHeight="10890" activeTab="1"/>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9495"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19140" windowHeight="8550"/>
   </bookViews>
   <sheets>
     <sheet name="Cards" sheetId="1" r:id="rId1"/>
@@ -18,10 +17,10 @@
     <sheet name="Original Cards" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Cards!$A$1:$H$95</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Cards!$A$1:$I$95</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Original Cards'!$A$1:$I$130</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1100" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1184" uniqueCount="356">
   <si>
     <t>Flask</t>
   </si>
@@ -845,12 +844,6 @@
     <t xml:space="preserve">Choose a player.  That player may discard a Corruption card </t>
   </si>
   <si>
-    <t>Combo Trigger</t>
-  </si>
-  <si>
-    <t>Physical</t>
-  </si>
-  <si>
     <t>Willpower</t>
   </si>
   <si>
@@ -909,9 +902,6 @@
   </si>
   <si>
     <t>Gain 1 :shield: and 2 :coin:</t>
-  </si>
-  <si>
-    <t>Combo Effect</t>
   </si>
   <si>
     <t>Look at any face down spawn</t>
@@ -1097,9 +1087,6 @@
     <t>Repair 3 damage from walls connected to your square</t>
   </si>
   <si>
-    <t>Repair another 1 damage from a wall connected to your square</t>
-  </si>
-  <si>
     <t>Total Unique Cards</t>
   </si>
   <si>
@@ -1137,12 +1124,33 @@
   </si>
   <si>
     <t>Action</t>
+  </si>
+  <si>
+    <t>ComboEffect</t>
+  </si>
+  <si>
+    <t>ComboTrigger</t>
+  </si>
+  <si>
+    <t>Repair 1 damage to a wall</t>
+  </si>
+  <si>
+    <t>Repair an additional 1 damage to a wall</t>
+  </si>
+  <si>
+    <t>Coop</t>
+  </si>
+  <si>
+    <t>IsCoop</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1198,7 +1206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1231,19 +1239,22 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1559,13 +1570,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I74"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:J95"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
-    </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1573,14 +1583,15 @@
     <col min="1" max="1" width="10.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="5.42578125" style="2" customWidth="1"/>
     <col min="3" max="3" width="20.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="41" style="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="31.42578125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="9.28515625" style="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="41" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="31.42578125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>12</v>
       </c>
@@ -1591,809 +1602,939 @@
         <v>8</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>354</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>256</v>
-      </c>
       <c r="G1" s="5" t="s">
-        <v>278</v>
+        <v>350</v>
       </c>
       <c r="H1" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
+    <row r="2" spans="1:10" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B2" s="2">
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>258</v>
-      </c>
+      <c r="D2" s="20"/>
       <c r="E2" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="I2" s="7"/>
-    </row>
-    <row r="3" spans="1:9" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
+      <c r="J2" s="7"/>
+    </row>
+    <row r="3" spans="1:10" s="9" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B3" s="2">
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>258</v>
+      <c r="D3" s="20" t="s">
+        <v>355</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>294</v>
-      </c>
       <c r="G3" s="1" t="s">
-        <v>336</v>
+        <v>291</v>
       </c>
       <c r="H3" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
+    <row r="4" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B4" s="2">
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>294</v>
+      <c r="D4" s="20" t="s">
+        <v>355</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>275</v>
+        <v>291</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>259</v>
+        <v>273</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
+    <row r="5" spans="1:10" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B5" s="2">
         <v>1</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>293</v>
-      </c>
+        <v>281</v>
+      </c>
+      <c r="D5" s="20"/>
       <c r="E5" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="1" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B6" s="2">
         <v>1</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>293</v>
-      </c>
+      <c r="D6" s="20"/>
       <c r="E6" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="F6" s="1"/>
+        <v>290</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>299</v>
+      </c>
       <c r="G6" s="1"/>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="1"/>
+      <c r="I6" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B7" s="2">
         <v>1</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>258</v>
-      </c>
       <c r="E7" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="G7" s="1" t="s">
-        <v>298</v>
+        <v>257</v>
       </c>
       <c r="H7" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B8" s="2">
         <v>1</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>293</v>
-      </c>
       <c r="E8" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B9" s="2">
         <v>1</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>294</v>
-      </c>
       <c r="E9" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="G9" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B10" s="2">
         <v>1</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="2">
-        <v>1</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>326</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B12" s="2">
-        <v>1</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="2">
-        <v>1</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>306</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="2">
-        <v>1</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="2">
-        <v>1</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>259</v>
+      <c r="D15" s="20" t="s">
+        <v>355</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>280</v>
+        <v>257</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>258</v>
+        <v>277</v>
       </c>
       <c r="G15" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="I15" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B16" s="2">
         <v>1</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>293</v>
+      <c r="D16" s="20" t="s">
+        <v>355</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>280</v>
+        <v>290</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>294</v>
+        <v>277</v>
       </c>
       <c r="G16" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="I16" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B17" s="2">
         <v>1</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>293</v>
-      </c>
       <c r="E17" s="1" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="G17" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="H17" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="I17" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B18" s="2">
         <v>1</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>258</v>
+        <v>274</v>
       </c>
       <c r="E18" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="G18" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="H18" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="H18" s="1" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18" s="1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B19" s="2">
         <v>1</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>294</v>
-      </c>
       <c r="E19" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>293</v>
-      </c>
       <c r="G19" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="H19" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="I19" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B20" s="2">
         <v>1</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>293</v>
+      <c r="D20" s="20" t="s">
+        <v>355</v>
       </c>
       <c r="E20" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>258</v>
-      </c>
       <c r="G20" s="1" t="s">
-        <v>308</v>
+        <v>256</v>
       </c>
       <c r="H20" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="I20" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B21" s="2">
         <v>1</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>307</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>259</v>
+        <v>304</v>
       </c>
       <c r="E21" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="G21" s="1" t="s">
-        <v>287</v>
+        <v>257</v>
       </c>
       <c r="H21" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="I21" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B22" s="10">
         <v>28</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>271</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>268</v>
-      </c>
+        <v>269</v>
+      </c>
+      <c r="D22" s="7"/>
       <c r="E22" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="F22" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H22" s="7"/>
+      <c r="I22" s="7" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B23" s="2">
         <v>1</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>294</v>
-      </c>
       <c r="E23" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>293</v>
-      </c>
       <c r="G23" s="1" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="H23" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="I23" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B24" s="2">
         <v>1</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>324</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>259</v>
+        <v>321</v>
+      </c>
+      <c r="D24" s="20" t="s">
+        <v>355</v>
       </c>
       <c r="E24" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>294</v>
-      </c>
       <c r="G24" s="1" t="s">
-        <v>279</v>
+        <v>291</v>
       </c>
       <c r="H24" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="I24" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B25" s="2">
         <v>1</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>258</v>
-      </c>
       <c r="E25" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="H25" s="1" t="s">
+      <c r="I25" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B26" s="2">
         <v>1</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>293</v>
-      </c>
       <c r="E26" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="F26" s="1" t="s">
-        <v>293</v>
-      </c>
       <c r="G26" s="1" t="s">
-        <v>273</v>
+        <v>290</v>
       </c>
       <c r="H26" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="I26" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B27" s="2">
         <v>1</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D27" s="1" t="s">
-        <v>259</v>
+      <c r="D27" s="20" t="s">
+        <v>355</v>
       </c>
       <c r="E27" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="F27" s="1" t="s">
-        <v>258</v>
-      </c>
       <c r="G27" s="1" t="s">
-        <v>337</v>
+        <v>256</v>
       </c>
       <c r="H27" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="I27" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B28" s="2">
         <v>1</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D28" s="1" t="s">
-        <v>293</v>
-      </c>
       <c r="E28" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>293</v>
-      </c>
       <c r="G28" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="H28" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="H28" s="1" t="s">
+      <c r="I28" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B29" s="2">
         <v>1</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>262</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>293</v>
+        <v>260</v>
       </c>
       <c r="E29" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="F29" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="F29" s="1" t="s">
-        <v>294</v>
-      </c>
       <c r="G29" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="H29" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="H29" s="1" t="s">
+      <c r="I29" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B30" s="2">
         <v>1</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>258</v>
+      <c r="D30" s="20" t="s">
+        <v>355</v>
       </c>
       <c r="E30" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="F30" s="1" t="s">
-        <v>293</v>
-      </c>
       <c r="G30" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="H30" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="H30" s="1" t="s">
+      <c r="I30" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B31" s="2">
         <v>1</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>293</v>
-      </c>
       <c r="E31" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="F31" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="F31" s="1" t="s">
-        <v>293</v>
-      </c>
       <c r="G31" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="H31" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="H31" s="1" t="s">
+      <c r="I31" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B32" s="2">
         <v>1</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="D32" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="E32" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="H32" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="I32" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B33" s="2">
         <v>1</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>294</v>
-      </c>
       <c r="E33" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="F33" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="F33" s="1" t="s">
-        <v>258</v>
-      </c>
       <c r="G33" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="H33" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="H33" s="1" t="s">
+      <c r="I33" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B34" s="2">
         <v>1</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>312</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>258</v>
+        <v>309</v>
       </c>
       <c r="E34" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="F34" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="F34" s="1" t="s">
-        <v>258</v>
-      </c>
       <c r="G34" s="1" t="s">
-        <v>280</v>
+        <v>256</v>
       </c>
       <c r="H34" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="I34" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B35" s="2">
         <v>1</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>325</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>259</v>
+        <v>322</v>
       </c>
       <c r="E35" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="F35" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="F35" s="1" t="s">
-        <v>258</v>
-      </c>
       <c r="G35" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="H35" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="H35" s="1" t="s">
+      <c r="I35" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B36" s="2">
         <v>1</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D36" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="E36" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="F36" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="F36" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="G36" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="H36" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="H36" s="1" t="s">
+      <c r="I36" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B37" s="2">
         <v>1</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="E37" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="F37" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="F37" s="1" t="s">
-        <v>294</v>
-      </c>
       <c r="G37" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="H37" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="H37" s="1" t="s">
+      <c r="I37" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B38" s="10">
         <v>3</v>
@@ -2401,768 +2542,917 @@
       <c r="C38" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D38" s="9" t="s">
-        <v>259</v>
-      </c>
+      <c r="D38" s="7"/>
       <c r="E38" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="F38" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="F38" s="9"/>
-      <c r="G38" s="9"/>
-      <c r="H38" s="9" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H38" s="9"/>
+      <c r="I38" s="9" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B39" s="10">
         <v>3</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>261</v>
-      </c>
-      <c r="D39" s="9" t="s">
-        <v>258</v>
-      </c>
+        <v>259</v>
+      </c>
+      <c r="D39" s="7"/>
       <c r="E39" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="F39" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="F39" s="9"/>
-      <c r="G39" s="9"/>
-      <c r="H39" s="9" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H39" s="9"/>
+      <c r="I39" s="9" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B40" s="10">
         <v>3</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>269</v>
-      </c>
-      <c r="D40" s="9" t="s">
-        <v>294</v>
-      </c>
+        <v>267</v>
+      </c>
+      <c r="D40" s="7"/>
       <c r="E40" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="F40" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="F40" s="9"/>
-      <c r="G40" s="9"/>
-      <c r="H40" s="9" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H40" s="9"/>
+      <c r="I40" s="9" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B41" s="10">
         <v>3</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="D41" s="9" t="s">
-        <v>293</v>
-      </c>
+        <v>268</v>
+      </c>
+      <c r="D41" s="7"/>
       <c r="E41" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="F41" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="F41" s="9"/>
-      <c r="G41" s="9"/>
-      <c r="H41" s="9" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H41" s="9"/>
+      <c r="I41" s="9" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B42" s="2">
         <v>1</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="D42" s="1" t="s">
-        <v>293</v>
-      </c>
       <c r="E42" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="F42" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="H42" s="1" t="s">
+      <c r="I42" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B43" s="2">
         <v>1</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D43" s="1" t="s">
-        <v>293</v>
-      </c>
       <c r="E43" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="F43" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="F43" s="1" t="s">
-        <v>294</v>
-      </c>
       <c r="G43" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="H43" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="H43" s="1" t="s">
+      <c r="I43" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B44" s="2">
         <v>1</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="D44" s="1" t="s">
-        <v>294</v>
-      </c>
       <c r="E44" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="F44" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="H44" s="1" t="s">
+      <c r="I44" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B45" s="2">
         <v>1</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D45" s="1" t="s">
-        <v>294</v>
-      </c>
       <c r="E45" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="F45" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="F45" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="G45" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="H45" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="H45" s="1" t="s">
+      <c r="I45" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B46" s="2">
         <v>1</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>293</v>
+        <v>278</v>
+      </c>
+      <c r="D46" s="20" t="s">
+        <v>355</v>
       </c>
       <c r="E46" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="F46" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="F46" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="G46" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="H46" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="H46" s="1" t="s">
+      <c r="I46" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B47" s="2">
         <v>1</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D47" s="1" t="s">
-        <v>294</v>
+      <c r="D47" s="20" t="s">
+        <v>355</v>
       </c>
       <c r="E47" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="F47" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="F47" s="1" t="s">
-        <v>258</v>
-      </c>
       <c r="G47" s="1" t="s">
-        <v>287</v>
+        <v>256</v>
       </c>
       <c r="H47" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="I47" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B48" s="2">
         <v>1</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="D48" s="1" t="s">
-        <v>258</v>
+      <c r="D48" s="20" t="s">
+        <v>355</v>
       </c>
       <c r="E48" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="F48" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="F48" s="1" t="s">
+      <c r="G48" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="G48" s="1" t="s">
-        <v>287</v>
-      </c>
       <c r="H48" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="I48" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="49" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B49" s="2">
         <v>1</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="D49" s="1" t="s">
-        <v>294</v>
-      </c>
       <c r="E49" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="F49" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="H49" s="1" t="s">
+      <c r="I49" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B50" s="2">
         <v>1</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="D50" s="1" t="s">
-        <v>294</v>
-      </c>
       <c r="E50" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="F50" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="H50" s="1" t="s">
+      <c r="I50" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B51" s="2">
         <v>1</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>328</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>293</v>
+        <v>325</v>
+      </c>
+      <c r="D51" s="20" t="s">
+        <v>355</v>
       </c>
       <c r="E51" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="F51" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="F51" s="1" t="s">
-        <v>294</v>
-      </c>
       <c r="G51" s="1" t="s">
-        <v>327</v>
+        <v>291</v>
       </c>
       <c r="H51" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="I51" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B52" s="2">
         <v>1</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="D52" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="E52" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="F52" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="F52" s="1" t="s">
-        <v>258</v>
-      </c>
       <c r="G52" s="1" t="s">
-        <v>297</v>
+        <v>256</v>
       </c>
       <c r="H52" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="I52" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B53" s="2">
         <v>1</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>259</v>
+        <v>279</v>
       </c>
       <c r="E53" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="F53" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="F53" s="1" t="s">
-        <v>258</v>
-      </c>
       <c r="G53" s="1" t="s">
-        <v>337</v>
+        <v>256</v>
       </c>
       <c r="H53" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="I53" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B54" s="2">
         <v>1</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="D54" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="E54" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="F54" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="F54" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="G54" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="H54" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="H54" s="1" t="s">
+      <c r="I54" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B55" s="2">
         <v>1</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="D55" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="E55" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="F55" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="H55" s="1" t="s">
+      <c r="I55" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B56" s="2">
         <v>1</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="D56" s="1" t="s">
-        <v>258</v>
-      </c>
       <c r="E56" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="F56" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="F56" s="1" t="s">
-        <v>294</v>
-      </c>
       <c r="G56" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="H56" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="H56" s="1" t="s">
+      <c r="I56" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B57" s="2">
         <v>1</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>311</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>259</v>
+        <v>308</v>
+      </c>
+      <c r="D57" s="20" t="s">
+        <v>355</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>273</v>
+        <v>257</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>293</v>
+        <v>271</v>
       </c>
       <c r="G57" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="H57" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="H57" s="1" t="s">
+      <c r="I57" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B58" s="2">
         <v>1</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="D58" s="1" t="s">
+      <c r="D58" s="20" t="s">
+        <v>355</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="H58" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="E58" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="H58" s="1" t="s">
+      <c r="I58" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B59" s="2">
         <v>1</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D59" s="1" t="s">
-        <v>258</v>
-      </c>
       <c r="E59" s="1" t="s">
-        <v>286</v>
+        <v>256</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>259</v>
+        <v>283</v>
       </c>
       <c r="G59" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="H59" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="H59" s="1" t="s">
+      <c r="I59" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="60" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B60" s="2">
         <v>1</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D60" s="1" t="s">
-        <v>294</v>
-      </c>
       <c r="E60" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="H60" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="I60" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="61" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B61" s="2">
         <v>1</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>313</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>258</v>
+        <v>310</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>295</v>
+        <v>256</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="G61" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="H61" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="H61" s="1" t="s">
+      <c r="I61" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="62" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B62" s="2">
         <v>1</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>293</v>
+        <v>280</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>258</v>
+        <v>292</v>
       </c>
       <c r="G62" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="H62" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="H62" s="1" t="s">
+      <c r="I62" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="63" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B63" s="2">
         <v>1</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>293</v>
+        <v>264</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="H63" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="I63" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="64" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B64" s="2">
         <v>1</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D64" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="E64" s="1" t="s">
-        <v>337</v>
+        <v>257</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>258</v>
+        <v>334</v>
       </c>
       <c r="G64" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="H64" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="H64" s="1" t="s">
+      <c r="I64" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="65" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B65" s="2">
         <v>1</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>274</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>258</v>
+        <v>272</v>
+      </c>
+      <c r="D65" s="20" t="s">
+        <v>355</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>337</v>
+        <v>256</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>259</v>
+        <v>334</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>339</v>
+        <v>257</v>
       </c>
       <c r="H65" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="I65" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="66" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B66" s="2">
         <v>1</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>259</v>
+        <v>331</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="H66" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="I66" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B67" s="2">
         <v>1</v>
       </c>
       <c r="C67" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="D67" s="1" t="s">
-        <v>294</v>
+      <c r="D67" s="20" t="s">
+        <v>355</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>341</v>
+        <v>290</v>
       </c>
       <c r="H67" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="I67" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="68" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B68" s="2">
         <v>1</v>
       </c>
       <c r="C68" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="D68" s="1" t="s">
-        <v>258</v>
-      </c>
       <c r="E68" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="F68" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="H68" s="1" t="s">
+      <c r="I68" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="69" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B69" s="2">
         <v>1</v>
       </c>
       <c r="C69" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="D69" s="1" t="s">
-        <v>258</v>
-      </c>
       <c r="E69" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="F69" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="H69" s="1" t="s">
+      <c r="I69" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="70" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B70" s="2">
         <v>1</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="H70" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="I70" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="71" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B71" s="2">
         <v>1</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>265</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="H71" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="I71" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="72" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B72" s="2">
         <v>1</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="H72" s="1" t="s">
+      <c r="F72" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="I72" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="73" spans="2:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B73" s="2">
         <v>1</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>289</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="H73" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="I73" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="74" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="B74" s="2">
         <v>1</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>309</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>293</v>
+        <v>306</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>310</v>
+        <v>290</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>293</v>
+        <v>307</v>
       </c>
       <c r="G74" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="H74" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="H74" s="1" t="s">
+      <c r="I74" s="1" t="s">
         <v>50</v>
       </c>
     </row>
+    <row r="75" spans="1:9" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="76" spans="1:9" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="77" spans="1:9" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="78" spans="1:9" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="79" spans="1:9" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="80" spans="1:9" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="81" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="82" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="83" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="84" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="85" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="86" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="87" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="88" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="89" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="90" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="91" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="92" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="93" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="94" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="95" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <autoFilter ref="A1:H95">
-    <sortState ref="A2:H130">
-      <sortCondition ref="D1:D130"/>
+  <autoFilter ref="A1:I95">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="Cunning"/>
+      </filters>
+    </filterColumn>
+    <sortState ref="A2:I130">
+      <sortCondition ref="E1:E130"/>
     </sortState>
   </autoFilter>
-  <sortState ref="A2:I74">
-    <sortCondition ref="E2:E74"/>
-    <sortCondition ref="G2:G74"/>
+  <sortState ref="A2:J74">
+    <sortCondition ref="F2:F74"/>
+    <sortCondition ref="H2:H74"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3174,12 +3464,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J42"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3187,937 +3474,989 @@
     <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>340</v>
-      </c>
-      <c r="B1" s="13">
+        <v>336</v>
+      </c>
+      <c r="B1" s="12">
         <f>COUNTA(Cards!C:C)-1</f>
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
-      <c r="B2" s="13"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="18" t="s">
-        <v>335</v>
-      </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
-        <v>322</v>
-      </c>
-      <c r="B4" s="16" t="s">
+      <c r="B2" s="12"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="15"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="19" t="s">
+        <v>332</v>
+      </c>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>312</v>
+      </c>
+      <c r="C4" s="15" t="s">
         <v>315</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="D4" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>317</v>
+      </c>
+      <c r="F4" s="15" t="s">
         <v>318</v>
       </c>
-      <c r="D4" s="16" t="s">
-        <v>319</v>
-      </c>
-      <c r="E4" s="16" t="s">
-        <v>320</v>
-      </c>
-      <c r="F4" s="16" t="s">
-        <v>321</v>
-      </c>
-      <c r="G4" s="16" t="s">
-        <v>330</v>
-      </c>
-      <c r="H4" s="16" t="s">
-        <v>332</v>
-      </c>
-      <c r="I4" s="16" t="s">
-        <v>264</v>
-      </c>
-      <c r="J4" s="16" t="s">
+      <c r="G4" s="15" t="s">
+        <v>327</v>
+      </c>
+      <c r="H4" s="15" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
-        <v>268</v>
-      </c>
-      <c r="B5" s="15">
-        <f>COUNTIF(Cards!D:D,"None")</f>
+      <c r="I4" s="15" t="s">
+        <v>262</v>
+      </c>
+      <c r="J4" s="15" t="s">
+        <v>326</v>
+      </c>
+      <c r="K4" s="15" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>266</v>
+      </c>
+      <c r="B5" s="14">
+        <f>COUNTIF(Cards!E:E,"None")</f>
         <v>1</v>
       </c>
       <c r="C5">
-        <f>COUNTIFS(Cards!D:D,"None", Cards!E:E, "*strike*")</f>
+        <f>COUNTIFS(Cards!E:E,"None", Cards!F:F, "*strike*")</f>
         <v>0</v>
       </c>
       <c r="D5">
-        <f>COUNTIFS(Cards!D:D,"None", Cards!E:E, "*move*")</f>
+        <f>COUNTIFS(Cards!E:E,"None", Cards!F:F, "*move*")</f>
         <v>0</v>
       </c>
       <c r="E5">
-        <f>COUNTIFS(Cards!D:D,"None", Cards!E:E, "*heart*")</f>
+        <f>COUNTIFS(Cards!E:E,"None", Cards!F:F, "*heart*")</f>
         <v>0</v>
       </c>
       <c r="F5">
-        <f>COUNTIFS(Cards!D:D,"None", Cards!E:E, "*coin*")</f>
+        <f>COUNTIFS(Cards!E:E,"None", Cards!F:F, "*coin*")</f>
         <v>1</v>
       </c>
       <c r="G5">
-        <f>COUNTIFS(Cards!D:D,"None", Cards!E:E, "*shield*")</f>
+        <f>COUNTIFS(Cards!E:E,"None", Cards!F:F, "*shield*")</f>
         <v>0</v>
       </c>
       <c r="H5">
-        <f>COUNTIFS(Cards!D:D,"None", Cards!E:E, "*draw*")</f>
+        <f>COUNTIFS(Cards!E:E,"None", Cards!F:F, "*draw*")</f>
         <v>0</v>
       </c>
       <c r="I5">
-        <f>COUNTIFS(Cards!D:D,"None", Cards!E:E, "*repair*")</f>
+        <f>COUNTIFS(Cards!E:E,"None", Cards!F:F, "*repair*")</f>
         <v>0</v>
       </c>
       <c r="J5">
         <f>B5-SUM(C5:H5)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5">
+        <f>COUNTIFS(Cards!E:E,"None", Cards!D:D, "*yes*")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>259</v>
-      </c>
-      <c r="B6" s="15">
-        <f>COUNTIF(Cards!D:D,"Strength")</f>
+        <v>257</v>
+      </c>
+      <c r="B6" s="14">
+        <f>COUNTIF(Cards!E:E,"Strength")</f>
         <v>18</v>
       </c>
       <c r="C6">
-        <f>COUNTIFS(Cards!D:D,"Strength", Cards!E:E, "*strike*")</f>
+        <f>COUNTIFS(Cards!E:E,"Strength", Cards!F:F, "*strike*")</f>
         <v>7</v>
       </c>
       <c r="D6">
-        <f>COUNTIFS(Cards!D:D,"Strength", Cards!E:E, "*move*")</f>
+        <f>COUNTIFS(Cards!E:E,"Strength", Cards!F:F, "*move*")</f>
         <v>1</v>
       </c>
       <c r="E6">
-        <f>COUNTIFS(Cards!D:D,"Strength", Cards!E:E, "*heart*")</f>
+        <f>COUNTIFS(Cards!E:E,"Strength", Cards!F:F, "*heart*")</f>
         <v>1</v>
       </c>
       <c r="F6">
-        <f>COUNTIFS(Cards!D:D,"Strength", Cards!E:E, "*coin*")</f>
+        <f>COUNTIFS(Cards!E:E,"Strength", Cards!F:F, "*coin*")</f>
         <v>2</v>
       </c>
       <c r="G6">
-        <f>COUNTIFS(Cards!D:D,"Strength", Cards!E:E, "*shield*")</f>
+        <f>COUNTIFS(Cards!E:E,"Strength", Cards!F:F, "*shield*")</f>
         <v>3</v>
       </c>
       <c r="H6">
-        <f>COUNTIFS(Cards!D:D,"Strength", Cards!E:E, "*draw*")</f>
+        <f>COUNTIFS(Cards!E:E,"Strength", Cards!F:F, "*draw*")</f>
         <v>1</v>
       </c>
       <c r="I6">
-        <f>COUNTIFS(Cards!D:D,"Strength", Cards!E:E, "*repair*")</f>
+        <f>COUNTIFS(Cards!E:E,"Strength", Cards!F:F, "*repair*")</f>
         <v>2</v>
       </c>
       <c r="J6">
         <f>B6-SUM(C6:H6)</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6">
+        <f>COUNTIFS(Cards!E:E,"Strength", Cards!D:D, "*yes*")</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>258</v>
-      </c>
-      <c r="B7" s="15">
-        <f>COUNTIF(Cards!D:D,"Willpower")</f>
+        <v>256</v>
+      </c>
+      <c r="B7" s="14">
+        <f>COUNTIF(Cards!E:E,"Willpower")</f>
         <v>18</v>
       </c>
       <c r="C7">
-        <f>COUNTIFS(Cards!D:D,"Willpower", Cards!E:E, "*strike*")</f>
+        <f>COUNTIFS(Cards!E:E,"Willpower", Cards!F:F, "*strike*")</f>
         <v>2</v>
       </c>
       <c r="D7">
-        <f>COUNTIFS(Cards!D:D,"Willpower", Cards!E:E, "*move*")</f>
+        <f>COUNTIFS(Cards!E:E,"Willpower", Cards!F:F, "*move*")</f>
         <v>0</v>
       </c>
       <c r="E7">
-        <f>COUNTIFS(Cards!D:D,"Willpower", Cards!E:E, "*heart*")</f>
+        <f>COUNTIFS(Cards!E:E,"Willpower", Cards!F:F, "*heart*")</f>
         <v>4</v>
       </c>
       <c r="F7">
-        <f>COUNTIFS(Cards!D:D,"Willpower", Cards!E:E, "*coin*")</f>
+        <f>COUNTIFS(Cards!E:E,"Willpower", Cards!F:F, "*coin*")</f>
         <v>3</v>
       </c>
       <c r="G7">
-        <f>COUNTIFS(Cards!D:D,"Willpower", Cards!E:E, "*shield*")</f>
+        <f>COUNTIFS(Cards!E:E,"Willpower", Cards!F:F, "*shield*")</f>
         <v>1</v>
       </c>
       <c r="H7">
-        <f>COUNTIFS(Cards!D:D,"Willpower", Cards!E:E, "*draw*")</f>
+        <f>COUNTIFS(Cards!E:E,"Willpower", Cards!F:F, "*draw*")</f>
         <v>3</v>
       </c>
       <c r="I7">
-        <f>COUNTIFS(Cards!D:D,"Willpower", Cards!E:E, "*repair*")</f>
+        <f>COUNTIFS(Cards!E:E,"Willpower", Cards!F:F, "*repair*")</f>
         <v>1</v>
       </c>
       <c r="J7">
         <f>B7-SUM(C7:H7)</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7">
+        <f>COUNTIFS(Cards!E:E,"Willpower", Cards!D:D, "*yes*")</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>293</v>
-      </c>
-      <c r="B8" s="15">
-        <f>COUNTIF(Cards!D:D,"Speed")</f>
+        <v>290</v>
+      </c>
+      <c r="B8" s="14">
+        <f>COUNTIF(Cards!E:E,"Speed")</f>
         <v>18</v>
       </c>
       <c r="C8">
-        <f>COUNTIFS(Cards!D:D,"Speed", Cards!E:E, "*strike*")</f>
+        <f>COUNTIFS(Cards!E:E,"Speed", Cards!F:F, "*strike*")</f>
         <v>5</v>
       </c>
       <c r="D8">
-        <f>COUNTIFS(Cards!D:D,"Speed", Cards!E:E, "*move*")</f>
+        <f>COUNTIFS(Cards!E:E,"Speed", Cards!F:F, "*move*")</f>
         <v>4</v>
       </c>
       <c r="E8">
-        <f>COUNTIFS(Cards!D:D,"Speed", Cards!E:E, "*heart*")</f>
+        <f>COUNTIFS(Cards!E:E,"Speed", Cards!F:F, "*heart*")</f>
         <v>3</v>
       </c>
       <c r="F8">
-        <f>COUNTIFS(Cards!D:D,"Speed", Cards!E:E, "*coin*")</f>
+        <f>COUNTIFS(Cards!E:E,"Speed", Cards!F:F, "*coin*")</f>
         <v>2</v>
       </c>
       <c r="G8">
-        <f>COUNTIFS(Cards!D:D,"Speed", Cards!E:E, "*shield*")</f>
+        <f>COUNTIFS(Cards!E:E,"Speed", Cards!F:F, "*shield*")</f>
         <v>2</v>
       </c>
       <c r="H8">
-        <f>COUNTIFS(Cards!D:D,"Speed", Cards!E:E, "*draw*")</f>
+        <f>COUNTIFS(Cards!E:E,"Speed", Cards!F:F, "*draw*")</f>
         <v>2</v>
       </c>
       <c r="I8">
-        <f>COUNTIFS(Cards!D:D,"Speed", Cards!E:E, "*repair*")</f>
+        <f>COUNTIFS(Cards!E:E,"Speed", Cards!F:F, "*repair*")</f>
         <v>0</v>
       </c>
       <c r="J8">
         <f>B8-SUM(C8:H8)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8">
+        <f>COUNTIFS(Cards!E:E,"Speed", Cards!D:D, "*yes*")</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>294</v>
-      </c>
-      <c r="B9" s="15">
-        <f>COUNTIF(Cards!D:D,"Cunning")</f>
+        <v>291</v>
+      </c>
+      <c r="B9" s="14">
+        <f>COUNTIF(Cards!E:E,"Cunning")</f>
         <v>18</v>
       </c>
       <c r="C9">
-        <f>COUNTIFS(Cards!D:D,"Cunning", Cards!E:E, "*strike*")</f>
+        <f>COUNTIFS(Cards!E:E,"Cunning", Cards!F:F, "*strike*")</f>
         <v>5</v>
       </c>
       <c r="D9">
-        <f>COUNTIFS(Cards!D:D,"Cunning", Cards!E:E, "*move*")</f>
+        <f>COUNTIFS(Cards!E:E,"Cunning", Cards!F:F, "*move*")</f>
         <v>0</v>
       </c>
       <c r="E9">
-        <f>COUNTIFS(Cards!D:D,"Cunning", Cards!E:E, "*heart*")</f>
+        <f>COUNTIFS(Cards!E:E,"Cunning", Cards!F:F, "*heart*")</f>
         <v>2</v>
       </c>
       <c r="F9">
-        <f>COUNTIFS(Cards!D:D,"Cunning", Cards!E:E, "*coin*")</f>
+        <f>COUNTIFS(Cards!E:E,"Cunning", Cards!F:F, "*coin*")</f>
         <v>5</v>
       </c>
       <c r="G9">
-        <f>COUNTIFS(Cards!D:D,"Cunning", Cards!E:E, "*shield*")</f>
+        <f>COUNTIFS(Cards!E:E,"Cunning", Cards!F:F, "*shield*")</f>
         <v>1</v>
       </c>
       <c r="H9">
-        <f>COUNTIFS(Cards!D:D,"Cunning", Cards!E:E, "*draw*")</f>
+        <f>COUNTIFS(Cards!E:E,"Cunning", Cards!F:F, "*draw*")</f>
         <v>3</v>
       </c>
       <c r="I9">
-        <f>COUNTIFS(Cards!D:D,"Cunning", Cards!E:E, "*repair*")</f>
+        <f>COUNTIFS(Cards!E:E,"Cunning", Cards!F:F, "*repair*")</f>
         <v>0</v>
       </c>
       <c r="J9">
         <f>B9-SUM(C9:H9)</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9">
+        <f>COUNTIFS(Cards!E:E,"Cunning", Cards!D:D, "*yes*")</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>315</v>
-      </c>
-      <c r="B10" s="15">
+        <v>312</v>
+      </c>
+      <c r="B10" s="14">
         <f>SUM(B5:B9)</f>
         <v>73</v>
       </c>
-      <c r="C10" s="15">
-        <f t="shared" ref="C10:J10" si="0">SUM(C5:C9)</f>
+      <c r="C10" s="14">
+        <f t="shared" ref="C10:K10" si="0">SUM(C5:C9)</f>
         <v>19</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="14">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="E10" s="15">
+      <c r="E10" s="14">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="F10" s="15">
+      <c r="F10" s="14">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="G10" s="15">
+      <c r="G10" s="14">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="H10" s="15">
+      <c r="H10" s="14">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="I10" s="15">
+      <c r="I10" s="14">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="J10" s="15">
+      <c r="J10" s="14">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="18" t="s">
-        <v>335</v>
-      </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
+      <c r="K10" s="14">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="15"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="19" t="s">
+        <v>332</v>
+      </c>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="19"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
+        <v>313</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>312</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>315</v>
+      </c>
+      <c r="D13" s="15" t="s">
         <v>316</v>
       </c>
-      <c r="B13" s="16" t="s">
-        <v>315</v>
-      </c>
-      <c r="C13" s="16" t="s">
+      <c r="E13" s="15" t="s">
+        <v>317</v>
+      </c>
+      <c r="F13" s="15" t="s">
         <v>318</v>
       </c>
-      <c r="D13" s="16" t="s">
-        <v>319</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>320</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>321</v>
-      </c>
-      <c r="G13" s="16" t="s">
-        <v>330</v>
-      </c>
-      <c r="H13" s="16" t="s">
-        <v>332</v>
-      </c>
-      <c r="I13" s="16" t="s">
-        <v>264</v>
-      </c>
-      <c r="J13" s="16" t="s">
+      <c r="G13" s="15" t="s">
+        <v>327</v>
+      </c>
+      <c r="H13" s="15" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I13" s="15" t="s">
+        <v>262</v>
+      </c>
+      <c r="J13" s="15" t="s">
+        <v>326</v>
+      </c>
+      <c r="K13" s="15" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>259</v>
-      </c>
-      <c r="B14" s="15">
-        <f>COUNTIF(Cards!F:F,"Strength")</f>
-        <v>11</v>
+        <v>257</v>
+      </c>
+      <c r="B14" s="14">
+        <f>COUNTIF(Cards!G:G,"Strength")</f>
+        <v>12</v>
       </c>
       <c r="C14">
-        <f>COUNTIFS(Cards!F:F,"Strength", Cards!G:G, "*strike*")</f>
+        <f>COUNTIFS(Cards!G:G,"Strength", Cards!H:H, "*strike*")</f>
         <v>6</v>
       </c>
       <c r="D14">
-        <f>COUNTIFS(Cards!F:F,"Strength", Cards!G:G, "*move*")</f>
+        <f>COUNTIFS(Cards!G:G,"Strength", Cards!H:H, "*move*")</f>
         <v>0</v>
       </c>
       <c r="E14">
-        <f>COUNTIFS(Cards!F:F,"Strength", Cards!G:G, "*heart*")</f>
+        <f>COUNTIFS(Cards!G:G,"Strength", Cards!H:H, "*heart*")</f>
         <v>1</v>
       </c>
       <c r="F14">
-        <f>COUNTIFS(Cards!F:F,"Strength", Cards!G:G, "*coin*")</f>
-        <v>1</v>
+        <f>COUNTIFS(Cards!G:G,"Strength", Cards!H:H, "*coin*")</f>
+        <v>2</v>
       </c>
       <c r="G14">
-        <f>COUNTIFS(Cards!F:F,"Strength", Cards!G:G, "*shield*")</f>
+        <f>COUNTIFS(Cards!G:G,"Strength", Cards!H:H, "*shield*")</f>
         <v>2</v>
       </c>
       <c r="H14">
-        <f>COUNTIFS(Cards!F:F,"Strength", Cards!G:G, "*draw*")</f>
+        <f>COUNTIFS(Cards!G:G,"Strength", Cards!H:H, "*draw*")</f>
         <v>0</v>
       </c>
       <c r="I14">
-        <f>COUNTIFS(Cards!F:F,"Strength", Cards!G:G, "*repair*")</f>
+        <f>COUNTIFS(Cards!G:G,"Strength", Cards!H:H, "*repair*")</f>
         <v>1</v>
       </c>
       <c r="J14">
         <f>B14-SUM(C14:H14)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K14">
+        <f>COUNTIFS(Cards!G:G,"Strength", Cards!D:D, "*yes*")</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>258</v>
-      </c>
-      <c r="B15" s="15">
-        <f>COUNTIF(Cards!F:F,"Willpower")</f>
+        <v>256</v>
+      </c>
+      <c r="B15" s="14">
+        <f>COUNTIF(Cards!G:G,"Willpower")</f>
         <v>11</v>
       </c>
       <c r="C15">
-        <f>COUNTIFS(Cards!F:F,"Willpower", Cards!G:G, "*strike*")</f>
+        <f>COUNTIFS(Cards!G:G,"Willpower", Cards!H:H, "*strike*")</f>
         <v>1</v>
       </c>
       <c r="D15">
-        <f>COUNTIFS(Cards!F:F,"Willpower", Cards!G:G, "*move*")</f>
+        <f>COUNTIFS(Cards!G:G,"Willpower", Cards!H:H, "*move*")</f>
         <v>0</v>
       </c>
       <c r="E15">
-        <f>COUNTIFS(Cards!F:F,"Willpower", Cards!G:G, "*heart*")</f>
+        <f>COUNTIFS(Cards!G:G,"Willpower", Cards!H:H, "*heart*")</f>
         <v>3</v>
       </c>
       <c r="F15">
-        <f>COUNTIFS(Cards!F:F,"Willpower", Cards!G:G, "*coin*")</f>
+        <f>COUNTIFS(Cards!G:G,"Willpower", Cards!H:H, "*coin*")</f>
         <v>3</v>
       </c>
       <c r="G15">
-        <f>COUNTIFS(Cards!F:F,"Willpower", Cards!G:G, "*shield*")</f>
+        <f>COUNTIFS(Cards!G:G,"Willpower", Cards!H:H, "*shield*")</f>
         <v>1</v>
       </c>
       <c r="H15">
-        <f>COUNTIFS(Cards!F:F,"Willpower", Cards!G:G, "*draw*")</f>
+        <f>COUNTIFS(Cards!G:G,"Willpower", Cards!H:H, "*draw*")</f>
         <v>1</v>
       </c>
       <c r="I15">
-        <f>COUNTIFS(Cards!F:F,"Willpower", Cards!G:G, "*repair*")</f>
+        <f>COUNTIFS(Cards!G:G,"Willpower", Cards!H:H, "*repair*")</f>
         <v>2</v>
       </c>
       <c r="J15">
         <f>B15-SUM(C15:H15)</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K15">
+        <f>COUNTIFS(Cards!G:G,"Willpower", Cards!D:D, "*yes*")</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>293</v>
-      </c>
-      <c r="B16" s="15">
-        <f>COUNTIF(Cards!F:F,"Speed")</f>
+        <v>290</v>
+      </c>
+      <c r="B16" s="14">
+        <f>COUNTIF(Cards!G:G,"Speed")</f>
         <v>11</v>
       </c>
       <c r="C16">
-        <f>COUNTIFS(Cards!F:F,"Speed", Cards!G:G, "*strike*")</f>
+        <f>COUNTIFS(Cards!G:G,"Speed", Cards!H:H, "*strike*")</f>
         <v>2</v>
       </c>
       <c r="D16">
-        <f>COUNTIFS(Cards!F:F,"Speed", Cards!G:G, "*move*")</f>
+        <f>COUNTIFS(Cards!G:G,"Speed", Cards!H:H, "*move*")</f>
         <v>4</v>
       </c>
       <c r="E16">
-        <f>COUNTIFS(Cards!F:F,"Speed", Cards!G:G, "*heart*")</f>
+        <f>COUNTIFS(Cards!G:G,"Speed", Cards!H:H, "*heart*")</f>
         <v>0</v>
       </c>
       <c r="F16">
-        <f>COUNTIFS(Cards!F:F,"Speed", Cards!G:G, "*coin*")</f>
+        <f>COUNTIFS(Cards!G:G,"Speed", Cards!H:H, "*coin*")</f>
         <v>2</v>
       </c>
       <c r="G16">
-        <f>COUNTIFS(Cards!F:F,"Speed", Cards!G:G, "*shield*")</f>
+        <f>COUNTIFS(Cards!G:G,"Speed", Cards!H:H, "*shield*")</f>
         <v>1</v>
       </c>
       <c r="H16">
-        <f>COUNTIFS(Cards!F:F,"Speed", Cards!G:G, "*draw*")</f>
+        <f>COUNTIFS(Cards!G:G,"Speed", Cards!H:H, "*draw*")</f>
         <v>0</v>
       </c>
       <c r="I16">
-        <f>COUNTIFS(Cards!F:F,"Speed", Cards!G:G, "*repair*")</f>
+        <f>COUNTIFS(Cards!G:G,"Speed", Cards!H:H, "*repair*")</f>
         <v>0</v>
       </c>
       <c r="J16">
         <f>B16-SUM(C16:H16)</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K16">
+        <f>COUNTIFS(Cards!G:G,"Speed", Cards!D:D, "*yes*")</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>294</v>
-      </c>
-      <c r="B17" s="15">
-        <f>COUNTIF(Cards!F:F,"Cunning")</f>
+        <v>291</v>
+      </c>
+      <c r="B17" s="14">
+        <f>COUNTIF(Cards!G:G,"Cunning")</f>
         <v>11</v>
       </c>
       <c r="C17">
-        <f>COUNTIFS(Cards!F:F,"Cunning", Cards!G:G, "*strike*")</f>
+        <f>COUNTIFS(Cards!G:G,"Cunning", Cards!H:H, "*strike*")</f>
         <v>2</v>
       </c>
       <c r="D17">
-        <f>COUNTIFS(Cards!F:F,"Cunning", Cards!G:G, "*move*")</f>
+        <f>COUNTIFS(Cards!G:G,"Cunning", Cards!H:H, "*move*")</f>
         <v>2</v>
       </c>
       <c r="E17">
-        <f>COUNTIFS(Cards!F:F,"Cunning", Cards!G:G, "*heart*")</f>
+        <f>COUNTIFS(Cards!G:G,"Cunning", Cards!H:H, "*heart*")</f>
         <v>1</v>
       </c>
       <c r="F17">
-        <f>COUNTIFS(Cards!F:F,"Cunning", Cards!G:G, "*coin*")</f>
+        <f>COUNTIFS(Cards!G:G,"Cunning", Cards!H:H, "*coin*")</f>
         <v>4</v>
       </c>
       <c r="G17">
-        <f>COUNTIFS(Cards!F:F,"Cunning", Cards!G:G, "*shield*")</f>
+        <f>COUNTIFS(Cards!G:G,"Cunning", Cards!H:H, "*shield*")</f>
         <v>0</v>
       </c>
       <c r="H17">
-        <f>COUNTIFS(Cards!F:F,"Cunning", Cards!G:G, "*draw*")</f>
+        <f>COUNTIFS(Cards!G:G,"Cunning", Cards!H:H, "*draw*")</f>
         <v>1</v>
       </c>
       <c r="I17">
-        <f>COUNTIFS(Cards!F:F,"Cunning", Cards!G:G, "*repair*")</f>
+        <f>COUNTIFS(Cards!G:G,"Cunning", Cards!H:H, "*repair*")</f>
         <v>0</v>
       </c>
       <c r="J17">
         <f>B17-SUM(C17:H17)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K17">
+        <f>COUNTIFS(Cards!G:G,"Cunning", Cards!D:D, "*yes*")</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>315</v>
-      </c>
-      <c r="B18" s="15">
+        <v>312</v>
+      </c>
+      <c r="B18" s="14">
         <f>SUM(B13:B17)</f>
-        <v>44</v>
-      </c>
-      <c r="C18" s="15">
+        <v>45</v>
+      </c>
+      <c r="C18" s="14">
         <f t="shared" ref="C18" si="1">SUM(C13:C17)</f>
         <v>11</v>
       </c>
-      <c r="D18" s="15">
+      <c r="D18" s="14">
         <f t="shared" ref="D18" si="2">SUM(D13:D17)</f>
         <v>6</v>
       </c>
-      <c r="E18" s="15">
+      <c r="E18" s="14">
         <f t="shared" ref="E18" si="3">SUM(E13:E17)</f>
         <v>5</v>
       </c>
-      <c r="F18" s="15">
+      <c r="F18" s="14">
         <f t="shared" ref="F18" si="4">SUM(F13:F17)</f>
-        <v>10</v>
-      </c>
-      <c r="G18" s="15">
+        <v>11</v>
+      </c>
+      <c r="G18" s="14">
         <f t="shared" ref="G18" si="5">SUM(G13:G17)</f>
         <v>4</v>
       </c>
-      <c r="H18" s="15">
+      <c r="H18" s="14">
         <f t="shared" ref="H18" si="6">SUM(H13:H17)</f>
         <v>2</v>
       </c>
-      <c r="I18" s="15">
+      <c r="I18" s="14">
         <f t="shared" ref="I18" si="7">SUM(I13:I17)</f>
         <v>3</v>
       </c>
-      <c r="J18" s="15">
-        <f t="shared" ref="J18" si="8">SUM(J13:J17)</f>
+      <c r="J18" s="14">
+        <f t="shared" ref="J18:K18" si="8">SUM(J13:J17)</f>
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K18" s="14">
+        <f>SUM(K13:K17)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="11"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C20" s="12" t="s">
-        <v>323</v>
-      </c>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C20" s="18" t="s">
+        <v>320</v>
+      </c>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
+        <v>314</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>312</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>257</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>256</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>290</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>315</v>
+      </c>
+      <c r="B22">
+        <f>COUNTIF(Cards!F:F,"*strike*")</f>
+        <v>19</v>
+      </c>
+      <c r="C22">
+        <f>COUNTIFS(Cards!F:F,"*strike*", Cards!E:E, "Strength")</f>
+        <v>7</v>
+      </c>
+      <c r="D22">
+        <f>COUNTIFS(Cards!F:F,"*strike*", Cards!E:E, "Willpower")</f>
+        <v>2</v>
+      </c>
+      <c r="E22">
+        <f>COUNTIFS(Cards!F:F,"*strike*", Cards!E:E, "Speed")</f>
+        <v>5</v>
+      </c>
+      <c r="F22">
+        <f>COUNTIFS(Cards!F:F,"*strike*", Cards!E:E, "Cunning")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>316</v>
+      </c>
+      <c r="B23">
+        <f>COUNTIF(Cards!F:F,"*move*")</f>
+        <v>5</v>
+      </c>
+      <c r="C23">
+        <f>COUNTIFS(Cards!F:F,"*move*", Cards!E:E, "Strength")</f>
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <f>COUNTIFS(Cards!F:F,"*move*", Cards!E:E, "Willpower")</f>
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <f>COUNTIFS(Cards!F:F,"*move*", Cards!E:E, "Speed")</f>
+        <v>4</v>
+      </c>
+      <c r="F23">
+        <f>COUNTIFS(Cards!F:F,"*move*", Cards!E:E, "Cunning")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>317</v>
       </c>
-      <c r="B21" s="11" t="s">
-        <v>315</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>259</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>258</v>
-      </c>
-      <c r="E21" s="11" t="s">
-        <v>293</v>
-      </c>
-      <c r="F21" s="11" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="B24">
+        <f>COUNTIF(Cards!F:F,"*heart*")</f>
+        <v>10</v>
+      </c>
+      <c r="C24">
+        <f>COUNTIFS(Cards!F:F,"*heart*", Cards!E:E, "Strength")</f>
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <f>COUNTIFS(Cards!F:F,"*heart*", Cards!E:E, "Willpower")</f>
+        <v>4</v>
+      </c>
+      <c r="E24">
+        <f>COUNTIFS(Cards!F:F,"*heart*", Cards!E:E, "Speed")</f>
+        <v>3</v>
+      </c>
+      <c r="F24">
+        <f>COUNTIFS(Cards!F:F,"*heart*", Cards!E:E, "Cunning")</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>318</v>
       </c>
-      <c r="B22">
-        <f>COUNTIF(Cards!E:E,"*strike*")</f>
-        <v>19</v>
-      </c>
-      <c r="C22">
-        <f>COUNTIFS(Cards!E:E,"*strike*", Cards!D:D, "Strength")</f>
+      <c r="B25">
+        <f>COUNTIF(Cards!F:F,"*coin*")</f>
+        <v>13</v>
+      </c>
+      <c r="C25">
+        <f>COUNTIFS(Cards!F:F,"*coin*", Cards!E:E, "Strength")</f>
+        <v>2</v>
+      </c>
+      <c r="D25">
+        <f>COUNTIFS(Cards!F:F,"*coin*", Cards!E:E, "Willpower")</f>
+        <v>3</v>
+      </c>
+      <c r="E25">
+        <f>COUNTIFS(Cards!F:F,"*coin*", Cards!E:E, "Speed")</f>
+        <v>2</v>
+      </c>
+      <c r="F25">
+        <f>COUNTIFS(Cards!F:F,"*coin*", Cards!E:E, "Cunning")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>327</v>
+      </c>
+      <c r="B26">
+        <f>COUNTIF(Cards!F:F,"*shield*")</f>
         <v>7</v>
       </c>
-      <c r="D22">
-        <f>COUNTIFS(Cards!E:E,"*strike*", Cards!D:D, "Willpower")</f>
+      <c r="C26">
+        <f>COUNTIFS(Cards!F:F,"*shield*", Cards!E:E, "Strength")</f>
+        <v>3</v>
+      </c>
+      <c r="D26">
+        <f>COUNTIFS(Cards!F:F,"*shield*", Cards!E:E, "Willpower")</f>
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <f>COUNTIFS(Cards!F:F,"*shield*", Cards!E:E, "Speed")</f>
         <v>2</v>
       </c>
-      <c r="E22">
-        <f>COUNTIFS(Cards!E:E,"*strike*", Cards!D:D, "Speed")</f>
-        <v>5</v>
-      </c>
-      <c r="F22">
-        <f>COUNTIFS(Cards!E:E,"*strike*", Cards!D:D, "Cunning")</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>319</v>
-      </c>
-      <c r="B23">
-        <f>COUNTIF(Cards!E:E,"*move*")</f>
-        <v>5</v>
-      </c>
-      <c r="C23">
-        <f>COUNTIFS(Cards!E:E,"*move*", Cards!D:D, "Strength")</f>
-        <v>1</v>
-      </c>
-      <c r="D23">
-        <f>COUNTIFS(Cards!E:E,"*move*", Cards!D:D, "Willpower")</f>
+      <c r="F26">
+        <f>COUNTIFS(Cards!F:F,"*shield*", Cards!E:E, "Cunning")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>329</v>
+      </c>
+      <c r="B27">
+        <f>COUNTIF(Cards!F:F,"*draw*")</f>
+        <v>9</v>
+      </c>
+      <c r="C27">
+        <f>COUNTIFS(Cards!F:F,"*draw*", Cards!E:E, "Strength")</f>
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <f>COUNTIFS(Cards!F:F,"*draw*", Cards!E:E, "Willpower")</f>
+        <v>3</v>
+      </c>
+      <c r="E27">
+        <f>COUNTIFS(Cards!F:F,"*draw*", Cards!E:E, "Speed")</f>
+        <v>2</v>
+      </c>
+      <c r="F27">
+        <f>COUNTIFS(Cards!F:F,"*draw*", Cards!E:E, "Cunning")</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>262</v>
+      </c>
+      <c r="B28">
+        <f>COUNTIF(Cards!F:F,"*repair*")</f>
+        <v>3</v>
+      </c>
+      <c r="C28">
+        <f>COUNTIFS(Cards!F:F,"*repair*", Cards!E:E, "Strength")</f>
+        <v>2</v>
+      </c>
+      <c r="D28">
+        <f>COUNTIFS(Cards!F:F,"*repair*", Cards!E:E, "Willpower")</f>
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <f>COUNTIFS(Cards!F:F,"*repair*", Cards!E:E, "Speed")</f>
         <v>0</v>
       </c>
-      <c r="E23">
-        <f>COUNTIFS(Cards!E:E,"*move*", Cards!D:D, "Speed")</f>
-        <v>4</v>
-      </c>
-      <c r="F23">
-        <f>COUNTIFS(Cards!E:E,"*move*", Cards!D:D, "Cunning")</f>
+      <c r="F28">
+        <f>COUNTIFS(Cards!F:F,"*repair*", Cards!E:E, "Cunning")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>320</v>
-      </c>
-      <c r="B24">
-        <f>COUNTIF(Cards!E:E,"*heart*")</f>
-        <v>10</v>
-      </c>
-      <c r="C24">
-        <f>COUNTIFS(Cards!E:E,"*heart*", Cards!D:D, "Strength")</f>
-        <v>1</v>
-      </c>
-      <c r="D24">
-        <f>COUNTIFS(Cards!E:E,"*heart*", Cards!D:D, "Willpower")</f>
-        <v>4</v>
-      </c>
-      <c r="E24">
-        <f>COUNTIFS(Cards!E:E,"*heart*", Cards!D:D, "Speed")</f>
-        <v>3</v>
-      </c>
-      <c r="F24">
-        <f>COUNTIFS(Cards!E:E,"*heart*", Cards!D:D, "Cunning")</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>321</v>
-      </c>
-      <c r="B25">
-        <f>COUNTIF(Cards!E:E,"*coin*")</f>
-        <v>13</v>
-      </c>
-      <c r="C25">
-        <f>COUNTIFS(Cards!E:E,"*coin*", Cards!D:D, "Strength")</f>
-        <v>2</v>
-      </c>
-      <c r="D25">
-        <f>COUNTIFS(Cards!E:E,"*coin*", Cards!D:D, "Willpower")</f>
-        <v>3</v>
-      </c>
-      <c r="E25">
-        <f>COUNTIFS(Cards!E:E,"*coin*", Cards!D:D, "Speed")</f>
-        <v>2</v>
-      </c>
-      <c r="F25">
-        <f>COUNTIFS(Cards!E:E,"*coin*", Cards!D:D, "Cunning")</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>330</v>
-      </c>
-      <c r="B26">
-        <f>COUNTIF(Cards!E:E,"*shield*")</f>
-        <v>7</v>
-      </c>
-      <c r="C26">
-        <f>COUNTIFS(Cards!E:E,"*shield*", Cards!D:D, "Strength")</f>
-        <v>3</v>
-      </c>
-      <c r="D26">
-        <f>COUNTIFS(Cards!E:E,"*shield*", Cards!D:D, "Willpower")</f>
-        <v>1</v>
-      </c>
-      <c r="E26">
-        <f>COUNTIFS(Cards!E:E,"*shield*", Cards!D:D, "Speed")</f>
-        <v>2</v>
-      </c>
-      <c r="F26">
-        <f>COUNTIFS(Cards!E:E,"*shield*", Cards!D:D, "Cunning")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>332</v>
-      </c>
-      <c r="B27">
-        <f>COUNTIF(Cards!E:E,"*draw*")</f>
-        <v>9</v>
-      </c>
-      <c r="C27">
-        <f>COUNTIFS(Cards!E:E,"*draw*", Cards!D:D, "Strength")</f>
-        <v>1</v>
-      </c>
-      <c r="D27">
-        <f>COUNTIFS(Cards!E:E,"*draw*", Cards!D:D, "Willpower")</f>
-        <v>3</v>
-      </c>
-      <c r="E27">
-        <f>COUNTIFS(Cards!E:E,"*draw*", Cards!D:D, "Speed")</f>
-        <v>2</v>
-      </c>
-      <c r="F27">
-        <f>COUNTIFS(Cards!E:E,"*draw*", Cards!D:D, "Cunning")</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>264</v>
-      </c>
-      <c r="B28">
-        <f>COUNTIF(Cards!E:E,"*repair*")</f>
-        <v>3</v>
-      </c>
-      <c r="C28">
-        <f>COUNTIFS(Cards!E:E,"*repair*", Cards!D:D, "Strength")</f>
-        <v>2</v>
-      </c>
-      <c r="D28">
-        <f>COUNTIFS(Cards!E:E,"*repair*", Cards!D:D, "Willpower")</f>
-        <v>1</v>
-      </c>
-      <c r="E28">
-        <f>COUNTIFS(Cards!E:E,"*repair*", Cards!D:D, "Speed")</f>
-        <v>0</v>
-      </c>
-      <c r="F28">
-        <f>COUNTIFS(Cards!E:E,"*repair*", Cards!D:D, "Cunning")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B29">
         <f>B1-SUM(B22:B27)</f>
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
+        <v>338</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>339</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>340</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>343</v>
+      </c>
+      <c r="E32" s="11" t="s">
         <v>342</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>343</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>344</v>
-      </c>
-      <c r="D32" s="11" t="s">
-        <v>347</v>
-      </c>
-      <c r="E32" s="11" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>318</v>
-      </c>
-      <c r="B33" s="19">
+        <v>315</v>
+      </c>
+      <c r="B33" s="17">
         <v>2</v>
       </c>
-      <c r="C33" s="19">
+      <c r="C33" s="17">
         <v>5</v>
       </c>
-      <c r="D33" s="19" t="s">
-        <v>348</v>
-      </c>
-      <c r="E33" s="19" t="s">
-        <v>349</v>
+      <c r="D33" s="17" t="s">
+        <v>344</v>
+      </c>
+      <c r="E33" s="17" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>319</v>
-      </c>
-      <c r="B34" s="19">
+        <v>316</v>
+      </c>
+      <c r="B34" s="17">
         <v>2</v>
       </c>
-      <c r="C34" s="19">
+      <c r="C34" s="17">
         <v>4</v>
       </c>
-      <c r="D34" s="19" t="s">
-        <v>348</v>
-      </c>
-      <c r="E34" s="19" t="s">
-        <v>349</v>
+      <c r="D34" s="17" t="s">
+        <v>344</v>
+      </c>
+      <c r="E34" s="17" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>320</v>
-      </c>
-      <c r="B35" s="19">
+        <v>317</v>
+      </c>
+      <c r="B35" s="17">
         <v>3</v>
       </c>
-      <c r="C35" s="19">
+      <c r="C35" s="17">
         <v>7</v>
       </c>
-      <c r="D35" s="19" t="s">
-        <v>348</v>
-      </c>
-      <c r="E35" s="19" t="s">
-        <v>349</v>
+      <c r="D35" s="17" t="s">
+        <v>344</v>
+      </c>
+      <c r="E35" s="17" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>321</v>
-      </c>
-      <c r="B36" s="19">
-        <v>1</v>
-      </c>
-      <c r="C36" s="19">
+        <v>318</v>
+      </c>
+      <c r="B36" s="17">
+        <v>1</v>
+      </c>
+      <c r="C36" s="17">
         <v>2</v>
       </c>
-      <c r="D36" s="19" t="s">
-        <v>348</v>
-      </c>
-      <c r="E36" s="19" t="s">
-        <v>349</v>
+      <c r="D36" s="17" t="s">
+        <v>344</v>
+      </c>
+      <c r="E36" s="17" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>330</v>
-      </c>
-      <c r="B37" s="19">
+        <v>327</v>
+      </c>
+      <c r="B37" s="17">
         <v>2</v>
       </c>
-      <c r="C37" s="19">
+      <c r="C37" s="17">
         <v>4</v>
       </c>
-      <c r="D37" s="19" t="s">
-        <v>348</v>
-      </c>
-      <c r="E37" s="19" t="s">
-        <v>349</v>
+      <c r="D37" s="17" t="s">
+        <v>344</v>
+      </c>
+      <c r="E37" s="17" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>332</v>
-      </c>
-      <c r="B38" s="19">
+        <v>329</v>
+      </c>
+      <c r="B38" s="17">
         <v>4</v>
       </c>
-      <c r="C38" s="19">
+      <c r="C38" s="17">
         <v>9</v>
       </c>
-      <c r="D38" s="19" t="s">
-        <v>348</v>
-      </c>
-      <c r="E38" s="19" t="s">
-        <v>349</v>
+      <c r="D38" s="17" t="s">
+        <v>344</v>
+      </c>
+      <c r="E38" s="17" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>264</v>
-      </c>
-      <c r="B39" s="19">
+        <v>262</v>
+      </c>
+      <c r="B39" s="17">
         <v>2</v>
       </c>
-      <c r="C39" s="19">
+      <c r="C39" s="17">
         <v>4</v>
       </c>
-      <c r="D39" s="19" t="s">
-        <v>348</v>
-      </c>
-      <c r="E39" s="19" t="s">
-        <v>349</v>
+      <c r="D39" s="17" t="s">
+        <v>344</v>
+      </c>
+      <c r="E39" s="17" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>352</v>
-      </c>
-      <c r="B40" s="19">
+        <v>348</v>
+      </c>
+      <c r="B40" s="17">
         <v>4</v>
       </c>
-      <c r="C40" s="19"/>
-      <c r="D40" s="19"/>
-      <c r="E40" s="19"/>
+      <c r="C40" s="17"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="17"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B42" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="C20:F20"/>
-    <mergeCell ref="C12:J12"/>
-    <mergeCell ref="C3:J3"/>
+    <mergeCell ref="C3:K3"/>
+    <mergeCell ref="C12:K12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4128,10 +4467,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I130"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>